<commit_message>
Commit ma gueule whoscored
</commit_message>
<xml_diff>
--- a/Résultats scraping.xlsx
+++ b/Résultats scraping.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16340" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -505,15 +505,10 @@
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -532,10 +527,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -815,8 +815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CB57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13:S13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="92" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -900,9 +900,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:80" x14ac:dyDescent="0.2">
-      <c r="A1" s="12"/>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
       <c r="D1">
         <v>1</v>
       </c>
@@ -1135,28 +1135,28 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:80" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:80" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="3" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:80" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1395,55 +1395,55 @@
       </c>
     </row>
     <row r="4" spans="1:80" x14ac:dyDescent="0.2">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="4" t="s">
         <v>80</v>
       </c>
       <c r="D4" t="s">
         <v>73</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="I4" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="J4" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="K4" s="14" t="s">
+      <c r="K4" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="L4" s="14" t="s">
+      <c r="L4" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="M4" s="14" t="s">
+      <c r="M4" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="N4" s="14" t="s">
+      <c r="N4" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="O4" s="14" t="s">
+      <c r="O4" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="P4" s="14" t="s">
+      <c r="P4" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="Q4" s="14" t="s">
+      <c r="Q4" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="R4" s="14" t="s">
+      <c r="R4" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="S4" s="14" t="s">
+      <c r="S4" s="5" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1456,807 +1456,839 @@
       </c>
     </row>
     <row r="6" spans="1:80" x14ac:dyDescent="0.2">
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
-      <c r="R6" s="3"/>
-      <c r="S6" s="4"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="13"/>
+      <c r="S6" s="14"/>
     </row>
     <row r="7" spans="1:80" x14ac:dyDescent="0.2">
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="6"/>
-      <c r="Q7" s="6"/>
-      <c r="R7" s="6"/>
-      <c r="S7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="8"/>
     </row>
     <row r="8" spans="1:80" x14ac:dyDescent="0.2">
-      <c r="D8" s="5"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="6"/>
-      <c r="S8" s="7"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="8"/>
     </row>
     <row r="9" spans="1:80" x14ac:dyDescent="0.2">
-      <c r="D9" s="5"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="6"/>
-      <c r="R9" s="6"/>
-      <c r="S9" s="7"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="8"/>
     </row>
     <row r="10" spans="1:80" x14ac:dyDescent="0.2">
-      <c r="D10" s="5"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="6"/>
-      <c r="S10" s="7"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="8"/>
     </row>
     <row r="11" spans="1:80" x14ac:dyDescent="0.2">
-      <c r="D11" s="5"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="6"/>
-      <c r="R11" s="6"/>
-      <c r="S11" s="7"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="8"/>
     </row>
     <row r="12" spans="1:80" x14ac:dyDescent="0.2">
-      <c r="D12" s="5"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
-      <c r="R12" s="6"/>
-      <c r="S12" s="7"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
+      <c r="S12" s="8"/>
     </row>
     <row r="13" spans="1:80" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="8"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="9"/>
-      <c r="Q13" s="9"/>
-      <c r="R13" s="9"/>
-      <c r="S13" s="10"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="10"/>
+      <c r="S13" s="11"/>
     </row>
     <row r="15" spans="1:80" x14ac:dyDescent="0.2">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="2" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:80" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E16" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="F16" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="G16" s="14" t="s">
+      <c r="G16" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="H16" s="14" t="s">
+      <c r="H16" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="I16" s="14" t="s">
+      <c r="I16" s="5" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
-      <c r="Q17" s="3"/>
-      <c r="R17" s="3"/>
-      <c r="S17" s="4"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="13"/>
+      <c r="P17" s="13"/>
+      <c r="Q17" s="13"/>
+      <c r="R17" s="13"/>
+      <c r="S17" s="14"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="D18" s="5"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="6"/>
-      <c r="O18" s="6"/>
-      <c r="P18" s="6"/>
-      <c r="Q18" s="6"/>
-      <c r="R18" s="6"/>
-      <c r="S18" s="7"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+      <c r="S18" s="8"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="D19" s="5"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="6"/>
-      <c r="P19" s="6"/>
-      <c r="Q19" s="6"/>
-      <c r="R19" s="6"/>
-      <c r="S19" s="7"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
+      <c r="S19" s="8"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="D20" s="5"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="6"/>
-      <c r="P20" s="6"/>
-      <c r="Q20" s="6"/>
-      <c r="R20" s="6"/>
-      <c r="S20" s="7"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
+      <c r="S20" s="8"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="D21" s="5"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="6"/>
-      <c r="O21" s="6"/>
-      <c r="P21" s="6"/>
-      <c r="Q21" s="6"/>
-      <c r="R21" s="6"/>
-      <c r="S21" s="7"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="7"/>
+      <c r="R21" s="7"/>
+      <c r="S21" s="8"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="D22" s="5"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6"/>
-      <c r="M22" s="6"/>
-      <c r="N22" s="6"/>
-      <c r="O22" s="6"/>
-      <c r="P22" s="6"/>
-      <c r="Q22" s="6"/>
-      <c r="R22" s="6"/>
-      <c r="S22" s="7"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
+      <c r="N22" s="7"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="7"/>
+      <c r="R22" s="7"/>
+      <c r="S22" s="8"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="D23" s="5"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
-      <c r="M23" s="6"/>
-      <c r="N23" s="6"/>
-      <c r="O23" s="6"/>
-      <c r="P23" s="6"/>
-      <c r="Q23" s="6"/>
-      <c r="R23" s="6"/>
-      <c r="S23" s="7"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="7"/>
+      <c r="P23" s="7"/>
+      <c r="Q23" s="7"/>
+      <c r="R23" s="7"/>
+      <c r="S23" s="8"/>
     </row>
     <row r="24" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D24" s="8"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
-      <c r="M24" s="9"/>
-      <c r="N24" s="9"/>
-      <c r="O24" s="9"/>
-      <c r="P24" s="9"/>
-      <c r="Q24" s="9"/>
-      <c r="R24" s="9"/>
-      <c r="S24" s="10"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="10"/>
+      <c r="R24" s="10"/>
+      <c r="S24" s="11"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="2" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="s">
+      <c r="A27" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="D27" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="E27" s="14" t="s">
+      <c r="E27" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="F27" s="14" t="s">
+      <c r="F27" s="5" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="D28" s="2"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
-      <c r="M28" s="3"/>
-      <c r="N28" s="3"/>
-      <c r="O28" s="3"/>
-      <c r="P28" s="3"/>
-      <c r="Q28" s="3"/>
-      <c r="R28" s="3"/>
-      <c r="S28" s="4"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="13"/>
+      <c r="N28" s="13"/>
+      <c r="O28" s="13"/>
+      <c r="P28" s="13"/>
+      <c r="Q28" s="13"/>
+      <c r="R28" s="13"/>
+      <c r="S28" s="14"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="D29" s="5"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6"/>
-      <c r="K29" s="6"/>
-      <c r="L29" s="6"/>
-      <c r="M29" s="6"/>
-      <c r="N29" s="6"/>
-      <c r="O29" s="6"/>
-      <c r="P29" s="6"/>
-      <c r="Q29" s="6"/>
-      <c r="R29" s="6"/>
-      <c r="S29" s="7"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="7"/>
+      <c r="N29" s="7"/>
+      <c r="O29" s="7"/>
+      <c r="P29" s="7"/>
+      <c r="Q29" s="7"/>
+      <c r="R29" s="7"/>
+      <c r="S29" s="8"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="D30" s="5"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="6"/>
-      <c r="K30" s="6"/>
-      <c r="L30" s="6"/>
-      <c r="M30" s="6"/>
-      <c r="N30" s="6"/>
-      <c r="O30" s="6"/>
-      <c r="P30" s="6"/>
-      <c r="Q30" s="6"/>
-      <c r="R30" s="6"/>
-      <c r="S30" s="7"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="7"/>
+      <c r="N30" s="7"/>
+      <c r="O30" s="7"/>
+      <c r="P30" s="7"/>
+      <c r="Q30" s="7"/>
+      <c r="R30" s="7"/>
+      <c r="S30" s="8"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="D31" s="5"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
-      <c r="K31" s="6"/>
-      <c r="L31" s="6"/>
-      <c r="M31" s="6"/>
-      <c r="N31" s="6"/>
-      <c r="O31" s="6"/>
-      <c r="P31" s="6"/>
-      <c r="Q31" s="6"/>
-      <c r="R31" s="6"/>
-      <c r="S31" s="7"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="7"/>
+      <c r="N31" s="7"/>
+      <c r="O31" s="7"/>
+      <c r="P31" s="7"/>
+      <c r="Q31" s="7"/>
+      <c r="R31" s="7"/>
+      <c r="S31" s="8"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="D32" s="5"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="6"/>
-      <c r="J32" s="6"/>
-      <c r="K32" s="6"/>
-      <c r="L32" s="6"/>
-      <c r="M32" s="6"/>
-      <c r="N32" s="6"/>
-      <c r="O32" s="6"/>
-      <c r="P32" s="6"/>
-      <c r="Q32" s="6"/>
-      <c r="R32" s="6"/>
-      <c r="S32" s="7"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="7"/>
+      <c r="L32" s="7"/>
+      <c r="M32" s="7"/>
+      <c r="N32" s="7"/>
+      <c r="O32" s="7"/>
+      <c r="P32" s="7"/>
+      <c r="Q32" s="7"/>
+      <c r="R32" s="7"/>
+      <c r="S32" s="8"/>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="D33" s="5"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
-      <c r="J33" s="6"/>
-      <c r="K33" s="6"/>
-      <c r="L33" s="6"/>
-      <c r="M33" s="6"/>
-      <c r="N33" s="6"/>
-      <c r="O33" s="6"/>
-      <c r="P33" s="6"/>
-      <c r="Q33" s="6"/>
-      <c r="R33" s="6"/>
-      <c r="S33" s="7"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="7"/>
+      <c r="P33" s="7"/>
+      <c r="Q33" s="7"/>
+      <c r="R33" s="7"/>
+      <c r="S33" s="8"/>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="D34" s="5"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6"/>
-      <c r="K34" s="6"/>
-      <c r="L34" s="6"/>
-      <c r="M34" s="6"/>
-      <c r="N34" s="6"/>
-      <c r="O34" s="6"/>
-      <c r="P34" s="6"/>
-      <c r="Q34" s="6"/>
-      <c r="R34" s="6"/>
-      <c r="S34" s="7"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
+      <c r="N34" s="7"/>
+      <c r="O34" s="7"/>
+      <c r="P34" s="7"/>
+      <c r="Q34" s="7"/>
+      <c r="R34" s="7"/>
+      <c r="S34" s="8"/>
     </row>
     <row r="35" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D35" s="8"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
-      <c r="I35" s="9"/>
-      <c r="J35" s="9"/>
-      <c r="K35" s="9"/>
-      <c r="L35" s="9"/>
-      <c r="M35" s="9"/>
-      <c r="N35" s="9"/>
-      <c r="O35" s="9"/>
-      <c r="P35" s="9"/>
-      <c r="Q35" s="9"/>
-      <c r="R35" s="9"/>
-      <c r="S35" s="10"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="10"/>
+      <c r="K35" s="10"/>
+      <c r="L35" s="10"/>
+      <c r="M35" s="10"/>
+      <c r="N35" s="10"/>
+      <c r="O35" s="10"/>
+      <c r="P35" s="10"/>
+      <c r="Q35" s="10"/>
+      <c r="R35" s="10"/>
+      <c r="S35" s="11"/>
     </row>
     <row r="38" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="11" t="s">
+      <c r="A38" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D38" s="14" t="s">
+      <c r="D38" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="E38" s="14" t="s">
+      <c r="E38" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="F38" s="14" t="s">
+      <c r="F38" s="5" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A39" s="13" t="s">
+      <c r="A39" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="D39" s="2"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
-      <c r="K39" s="3"/>
-      <c r="L39" s="3"/>
-      <c r="M39" s="3"/>
-      <c r="N39" s="3"/>
-      <c r="O39" s="3"/>
-      <c r="P39" s="3"/>
-      <c r="Q39" s="3"/>
-      <c r="R39" s="3"/>
-      <c r="S39" s="4"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13"/>
+      <c r="I39" s="13"/>
+      <c r="J39" s="13"/>
+      <c r="K39" s="13"/>
+      <c r="L39" s="13"/>
+      <c r="M39" s="13"/>
+      <c r="N39" s="13"/>
+      <c r="O39" s="13"/>
+      <c r="P39" s="13"/>
+      <c r="Q39" s="13"/>
+      <c r="R39" s="13"/>
+      <c r="S39" s="14"/>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="D40" s="5"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
-      <c r="H40" s="6"/>
-      <c r="I40" s="6"/>
-      <c r="J40" s="6"/>
-      <c r="K40" s="6"/>
-      <c r="L40" s="6"/>
-      <c r="M40" s="6"/>
-      <c r="N40" s="6"/>
-      <c r="O40" s="6"/>
-      <c r="P40" s="6"/>
-      <c r="Q40" s="6"/>
-      <c r="R40" s="6"/>
-      <c r="S40" s="7"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="7"/>
+      <c r="K40" s="7"/>
+      <c r="L40" s="7"/>
+      <c r="M40" s="7"/>
+      <c r="N40" s="7"/>
+      <c r="O40" s="7"/>
+      <c r="P40" s="7"/>
+      <c r="Q40" s="7"/>
+      <c r="R40" s="7"/>
+      <c r="S40" s="8"/>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="D41" s="5"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
-      <c r="H41" s="6"/>
-      <c r="I41" s="6"/>
-      <c r="J41" s="6"/>
-      <c r="K41" s="6"/>
-      <c r="L41" s="6"/>
-      <c r="M41" s="6"/>
-      <c r="N41" s="6"/>
-      <c r="O41" s="6"/>
-      <c r="P41" s="6"/>
-      <c r="Q41" s="6"/>
-      <c r="R41" s="6"/>
-      <c r="S41" s="7"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="7"/>
+      <c r="J41" s="7"/>
+      <c r="K41" s="7"/>
+      <c r="L41" s="7"/>
+      <c r="M41" s="7"/>
+      <c r="N41" s="7"/>
+      <c r="O41" s="7"/>
+      <c r="P41" s="7"/>
+      <c r="Q41" s="7"/>
+      <c r="R41" s="7"/>
+      <c r="S41" s="8"/>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="D42" s="5"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
-      <c r="H42" s="6"/>
-      <c r="I42" s="6"/>
-      <c r="J42" s="6"/>
-      <c r="K42" s="6"/>
-      <c r="L42" s="6"/>
-      <c r="M42" s="6"/>
-      <c r="N42" s="6"/>
-      <c r="O42" s="6"/>
-      <c r="P42" s="6"/>
-      <c r="Q42" s="6"/>
-      <c r="R42" s="6"/>
-      <c r="S42" s="7"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="7"/>
+      <c r="J42" s="7"/>
+      <c r="K42" s="7"/>
+      <c r="L42" s="7"/>
+      <c r="M42" s="7"/>
+      <c r="N42" s="7"/>
+      <c r="O42" s="7"/>
+      <c r="P42" s="7"/>
+      <c r="Q42" s="7"/>
+      <c r="R42" s="7"/>
+      <c r="S42" s="8"/>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="D43" s="5"/>
-      <c r="E43" s="6"/>
-      <c r="F43" s="6"/>
-      <c r="G43" s="6"/>
-      <c r="H43" s="6"/>
-      <c r="I43" s="6"/>
-      <c r="J43" s="6"/>
-      <c r="K43" s="6"/>
-      <c r="L43" s="6"/>
-      <c r="M43" s="6"/>
-      <c r="N43" s="6"/>
-      <c r="O43" s="6"/>
-      <c r="P43" s="6"/>
-      <c r="Q43" s="6"/>
-      <c r="R43" s="6"/>
-      <c r="S43" s="7"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="7"/>
+      <c r="J43" s="7"/>
+      <c r="K43" s="7"/>
+      <c r="L43" s="7"/>
+      <c r="M43" s="7"/>
+      <c r="N43" s="7"/>
+      <c r="O43" s="7"/>
+      <c r="P43" s="7"/>
+      <c r="Q43" s="7"/>
+      <c r="R43" s="7"/>
+      <c r="S43" s="8"/>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="D44" s="5"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="6"/>
-      <c r="G44" s="6"/>
-      <c r="H44" s="6"/>
-      <c r="I44" s="6"/>
-      <c r="J44" s="6"/>
-      <c r="K44" s="6"/>
-      <c r="L44" s="6"/>
-      <c r="M44" s="6"/>
-      <c r="N44" s="6"/>
-      <c r="O44" s="6"/>
-      <c r="P44" s="6"/>
-      <c r="Q44" s="6"/>
-      <c r="R44" s="6"/>
-      <c r="S44" s="7"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
+      <c r="I44" s="7"/>
+      <c r="J44" s="7"/>
+      <c r="K44" s="7"/>
+      <c r="L44" s="7"/>
+      <c r="M44" s="7"/>
+      <c r="N44" s="7"/>
+      <c r="O44" s="7"/>
+      <c r="P44" s="7"/>
+      <c r="Q44" s="7"/>
+      <c r="R44" s="7"/>
+      <c r="S44" s="8"/>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="D45" s="5"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
-      <c r="G45" s="6"/>
-      <c r="H45" s="6"/>
-      <c r="I45" s="6"/>
-      <c r="J45" s="6"/>
-      <c r="K45" s="6"/>
-      <c r="L45" s="6"/>
-      <c r="M45" s="6"/>
-      <c r="N45" s="6"/>
-      <c r="O45" s="6"/>
-      <c r="P45" s="6"/>
-      <c r="Q45" s="6"/>
-      <c r="R45" s="6"/>
-      <c r="S45" s="7"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="7"/>
+      <c r="I45" s="7"/>
+      <c r="J45" s="7"/>
+      <c r="K45" s="7"/>
+      <c r="L45" s="7"/>
+      <c r="M45" s="7"/>
+      <c r="N45" s="7"/>
+      <c r="O45" s="7"/>
+      <c r="P45" s="7"/>
+      <c r="Q45" s="7"/>
+      <c r="R45" s="7"/>
+      <c r="S45" s="8"/>
     </row>
     <row r="46" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D46" s="8"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="9"/>
-      <c r="H46" s="9"/>
-      <c r="I46" s="9"/>
-      <c r="J46" s="9"/>
-      <c r="K46" s="9"/>
-      <c r="L46" s="9"/>
-      <c r="M46" s="9"/>
-      <c r="N46" s="9"/>
-      <c r="O46" s="9"/>
-      <c r="P46" s="9"/>
-      <c r="Q46" s="9"/>
-      <c r="R46" s="9"/>
-      <c r="S46" s="10"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="10"/>
+      <c r="H46" s="10"/>
+      <c r="I46" s="10"/>
+      <c r="J46" s="10"/>
+      <c r="K46" s="10"/>
+      <c r="L46" s="10"/>
+      <c r="M46" s="10"/>
+      <c r="N46" s="10"/>
+      <c r="O46" s="10"/>
+      <c r="P46" s="10"/>
+      <c r="Q46" s="10"/>
+      <c r="R46" s="10"/>
+      <c r="S46" s="11"/>
     </row>
     <row r="49" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="11" t="s">
+      <c r="A49" s="2" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A50" s="13" t="s">
+      <c r="A50" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="D50" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
-      <c r="G50" s="3"/>
-      <c r="H50" s="3"/>
-      <c r="I50" s="3"/>
-      <c r="J50" s="3"/>
-      <c r="K50" s="3"/>
-      <c r="L50" s="3"/>
-      <c r="M50" s="3"/>
-      <c r="N50" s="3"/>
-      <c r="O50" s="3"/>
-      <c r="P50" s="3"/>
-      <c r="Q50" s="3"/>
-      <c r="R50" s="3"/>
-      <c r="S50" s="4"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
+      <c r="H50" s="13"/>
+      <c r="I50" s="13"/>
+      <c r="J50" s="13"/>
+      <c r="K50" s="13"/>
+      <c r="L50" s="13"/>
+      <c r="M50" s="13"/>
+      <c r="N50" s="13"/>
+      <c r="O50" s="13"/>
+      <c r="P50" s="13"/>
+      <c r="Q50" s="13"/>
+      <c r="R50" s="13"/>
+      <c r="S50" s="14"/>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="D51" s="5"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="6"/>
-      <c r="G51" s="6"/>
-      <c r="H51" s="6"/>
-      <c r="I51" s="6"/>
-      <c r="J51" s="6"/>
-      <c r="K51" s="6"/>
-      <c r="L51" s="6"/>
-      <c r="M51" s="6"/>
-      <c r="N51" s="6"/>
-      <c r="O51" s="6"/>
-      <c r="P51" s="6"/>
-      <c r="Q51" s="6"/>
-      <c r="R51" s="6"/>
-      <c r="S51" s="7"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="7"/>
+      <c r="H51" s="7"/>
+      <c r="I51" s="7"/>
+      <c r="J51" s="7"/>
+      <c r="K51" s="7"/>
+      <c r="L51" s="7"/>
+      <c r="M51" s="7"/>
+      <c r="N51" s="7"/>
+      <c r="O51" s="7"/>
+      <c r="P51" s="7"/>
+      <c r="Q51" s="7"/>
+      <c r="R51" s="7"/>
+      <c r="S51" s="8"/>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="D52" s="5"/>
-      <c r="E52" s="6"/>
-      <c r="F52" s="6"/>
-      <c r="G52" s="6"/>
-      <c r="H52" s="6"/>
-      <c r="I52" s="6"/>
-      <c r="J52" s="6"/>
-      <c r="K52" s="6"/>
-      <c r="L52" s="6"/>
-      <c r="M52" s="6"/>
-      <c r="N52" s="6"/>
-      <c r="O52" s="6"/>
-      <c r="P52" s="6"/>
-      <c r="Q52" s="6"/>
-      <c r="R52" s="6"/>
-      <c r="S52" s="7"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="7"/>
+      <c r="G52" s="7"/>
+      <c r="H52" s="7"/>
+      <c r="I52" s="7"/>
+      <c r="J52" s="7"/>
+      <c r="K52" s="7"/>
+      <c r="L52" s="7"/>
+      <c r="M52" s="7"/>
+      <c r="N52" s="7"/>
+      <c r="O52" s="7"/>
+      <c r="P52" s="7"/>
+      <c r="Q52" s="7"/>
+      <c r="R52" s="7"/>
+      <c r="S52" s="8"/>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="D53" s="5"/>
-      <c r="E53" s="6"/>
-      <c r="F53" s="6"/>
-      <c r="G53" s="6"/>
-      <c r="H53" s="6"/>
-      <c r="I53" s="6"/>
-      <c r="J53" s="6"/>
-      <c r="K53" s="6"/>
-      <c r="L53" s="6"/>
-      <c r="M53" s="6"/>
-      <c r="N53" s="6"/>
-      <c r="O53" s="6"/>
-      <c r="P53" s="6"/>
-      <c r="Q53" s="6"/>
-      <c r="R53" s="6"/>
-      <c r="S53" s="7"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="7"/>
+      <c r="G53" s="7"/>
+      <c r="H53" s="7"/>
+      <c r="I53" s="7"/>
+      <c r="J53" s="7"/>
+      <c r="K53" s="7"/>
+      <c r="L53" s="7"/>
+      <c r="M53" s="7"/>
+      <c r="N53" s="7"/>
+      <c r="O53" s="7"/>
+      <c r="P53" s="7"/>
+      <c r="Q53" s="7"/>
+      <c r="R53" s="7"/>
+      <c r="S53" s="8"/>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="D54" s="5"/>
-      <c r="E54" s="6"/>
-      <c r="F54" s="6"/>
-      <c r="G54" s="6"/>
-      <c r="H54" s="6"/>
-      <c r="I54" s="6"/>
-      <c r="J54" s="6"/>
-      <c r="K54" s="6"/>
-      <c r="L54" s="6"/>
-      <c r="M54" s="6"/>
-      <c r="N54" s="6"/>
-      <c r="O54" s="6"/>
-      <c r="P54" s="6"/>
-      <c r="Q54" s="6"/>
-      <c r="R54" s="6"/>
-      <c r="S54" s="7"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="7"/>
+      <c r="G54" s="7"/>
+      <c r="H54" s="7"/>
+      <c r="I54" s="7"/>
+      <c r="J54" s="7"/>
+      <c r="K54" s="7"/>
+      <c r="L54" s="7"/>
+      <c r="M54" s="7"/>
+      <c r="N54" s="7"/>
+      <c r="O54" s="7"/>
+      <c r="P54" s="7"/>
+      <c r="Q54" s="7"/>
+      <c r="R54" s="7"/>
+      <c r="S54" s="8"/>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="D55" s="5"/>
-      <c r="E55" s="6"/>
-      <c r="F55" s="6"/>
-      <c r="G55" s="6"/>
-      <c r="H55" s="6"/>
-      <c r="I55" s="6"/>
-      <c r="J55" s="6"/>
-      <c r="K55" s="6"/>
-      <c r="L55" s="6"/>
-      <c r="M55" s="6"/>
-      <c r="N55" s="6"/>
-      <c r="O55" s="6"/>
-      <c r="P55" s="6"/>
-      <c r="Q55" s="6"/>
-      <c r="R55" s="6"/>
-      <c r="S55" s="7"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="7"/>
+      <c r="H55" s="7"/>
+      <c r="I55" s="7"/>
+      <c r="J55" s="7"/>
+      <c r="K55" s="7"/>
+      <c r="L55" s="7"/>
+      <c r="M55" s="7"/>
+      <c r="N55" s="7"/>
+      <c r="O55" s="7"/>
+      <c r="P55" s="7"/>
+      <c r="Q55" s="7"/>
+      <c r="R55" s="7"/>
+      <c r="S55" s="8"/>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="D56" s="5"/>
-      <c r="E56" s="6"/>
-      <c r="F56" s="6"/>
-      <c r="G56" s="6"/>
-      <c r="H56" s="6"/>
-      <c r="I56" s="6"/>
-      <c r="J56" s="6"/>
-      <c r="K56" s="6"/>
-      <c r="L56" s="6"/>
-      <c r="M56" s="6"/>
-      <c r="N56" s="6"/>
-      <c r="O56" s="6"/>
-      <c r="P56" s="6"/>
-      <c r="Q56" s="6"/>
-      <c r="R56" s="6"/>
-      <c r="S56" s="7"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="7"/>
+      <c r="F56" s="7"/>
+      <c r="G56" s="7"/>
+      <c r="H56" s="7"/>
+      <c r="I56" s="7"/>
+      <c r="J56" s="7"/>
+      <c r="K56" s="7"/>
+      <c r="L56" s="7"/>
+      <c r="M56" s="7"/>
+      <c r="N56" s="7"/>
+      <c r="O56" s="7"/>
+      <c r="P56" s="7"/>
+      <c r="Q56" s="7"/>
+      <c r="R56" s="7"/>
+      <c r="S56" s="8"/>
     </row>
     <row r="57" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D57" s="8"/>
-      <c r="E57" s="9"/>
-      <c r="F57" s="9"/>
-      <c r="G57" s="9"/>
-      <c r="H57" s="9"/>
-      <c r="I57" s="9"/>
-      <c r="J57" s="9"/>
-      <c r="K57" s="9"/>
-      <c r="L57" s="9"/>
-      <c r="M57" s="9"/>
-      <c r="N57" s="9"/>
-      <c r="O57" s="9"/>
-      <c r="P57" s="9"/>
-      <c r="Q57" s="9"/>
-      <c r="R57" s="9"/>
-      <c r="S57" s="10"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="10"/>
+      <c r="F57" s="10"/>
+      <c r="G57" s="10"/>
+      <c r="H57" s="10"/>
+      <c r="I57" s="10"/>
+      <c r="J57" s="10"/>
+      <c r="K57" s="10"/>
+      <c r="L57" s="10"/>
+      <c r="M57" s="10"/>
+      <c r="N57" s="10"/>
+      <c r="O57" s="10"/>
+      <c r="P57" s="10"/>
+      <c r="Q57" s="10"/>
+      <c r="R57" s="10"/>
+      <c r="S57" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D11:S11"/>
+    <mergeCell ref="D12:S12"/>
+    <mergeCell ref="D13:S13"/>
+    <mergeCell ref="D6:S6"/>
+    <mergeCell ref="D7:S7"/>
+    <mergeCell ref="D8:S8"/>
+    <mergeCell ref="D9:S9"/>
+    <mergeCell ref="D10:S10"/>
+    <mergeCell ref="D31:S31"/>
+    <mergeCell ref="D17:S17"/>
+    <mergeCell ref="D18:S18"/>
+    <mergeCell ref="D19:S19"/>
+    <mergeCell ref="D20:S20"/>
+    <mergeCell ref="D21:S21"/>
+    <mergeCell ref="D22:S22"/>
+    <mergeCell ref="D23:S23"/>
+    <mergeCell ref="D24:S24"/>
+    <mergeCell ref="D28:S28"/>
+    <mergeCell ref="D29:S29"/>
+    <mergeCell ref="D30:S30"/>
+    <mergeCell ref="D46:S46"/>
+    <mergeCell ref="D32:S32"/>
+    <mergeCell ref="D33:S33"/>
+    <mergeCell ref="D34:S34"/>
+    <mergeCell ref="D35:S35"/>
+    <mergeCell ref="D39:S39"/>
+    <mergeCell ref="D40:S40"/>
+    <mergeCell ref="D41:S41"/>
+    <mergeCell ref="D42:S42"/>
+    <mergeCell ref="D43:S43"/>
+    <mergeCell ref="D44:S44"/>
+    <mergeCell ref="D45:S45"/>
     <mergeCell ref="D56:S56"/>
     <mergeCell ref="D57:S57"/>
     <mergeCell ref="D50:S50"/>
@@ -2265,38 +2297,6 @@
     <mergeCell ref="D53:S53"/>
     <mergeCell ref="D54:S54"/>
     <mergeCell ref="D55:S55"/>
-    <mergeCell ref="D41:S41"/>
-    <mergeCell ref="D42:S42"/>
-    <mergeCell ref="D43:S43"/>
-    <mergeCell ref="D44:S44"/>
-    <mergeCell ref="D45:S45"/>
-    <mergeCell ref="D46:S46"/>
-    <mergeCell ref="D32:S32"/>
-    <mergeCell ref="D33:S33"/>
-    <mergeCell ref="D34:S34"/>
-    <mergeCell ref="D35:S35"/>
-    <mergeCell ref="D39:S39"/>
-    <mergeCell ref="D40:S40"/>
-    <mergeCell ref="D23:S23"/>
-    <mergeCell ref="D24:S24"/>
-    <mergeCell ref="D28:S28"/>
-    <mergeCell ref="D29:S29"/>
-    <mergeCell ref="D30:S30"/>
-    <mergeCell ref="D31:S31"/>
-    <mergeCell ref="D17:S17"/>
-    <mergeCell ref="D18:S18"/>
-    <mergeCell ref="D19:S19"/>
-    <mergeCell ref="D20:S20"/>
-    <mergeCell ref="D21:S21"/>
-    <mergeCell ref="D22:S22"/>
-    <mergeCell ref="D6:S6"/>
-    <mergeCell ref="D7:S7"/>
-    <mergeCell ref="D8:S8"/>
-    <mergeCell ref="D9:S9"/>
-    <mergeCell ref="D10:S10"/>
-    <mergeCell ref="D11:S11"/>
-    <mergeCell ref="D12:S12"/>
-    <mergeCell ref="D13:S13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>